<commit_message>
Casos de pruebas para los servicios soap
</commit_message>
<xml_diff>
--- a/Plan de calidad.xlsx
+++ b/Plan de calidad.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eros Adarraga\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eros Adarraga\Desktop\QA\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F29F0E9-FACD-4AB1-B0E1-258DB5F5ADEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009BE63A-B832-44F4-8D03-8412128A47DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="116">
   <si>
     <t xml:space="preserve">Area </t>
   </si>
@@ -443,15 +443,39 @@
   <si>
     <t>Cerrado</t>
   </si>
+  <si>
+    <t>Service soap contryInfo y SoapDemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se desea poder odtener informacion mediantes estos servicios soap para trabajar con los datos de paises y usuarios  en la aplicación que se esta contruyendo con los requerimientos necesarios </t>
+  </si>
+  <si>
+    <t xml:space="preserve">El alcance de las pruebas de los servicios soap sera garantizar el funcionamiento del proceso de cosultar codigo ISO por nombre, cosultar codigo de moneda por codigo ISO y buscar persona por ID .
+ Este alcance incluye las pruebas de diferentes ecenarios y componentes involucreados el los procesos de consulta en los servicios soap con la herrramienta SoapIU                                                                                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las  pruebas de seguridad no se tendran presente, Aunque el servicio SOAP pueda requerir autenticación y autorización, es posible que se necesiten pruebas adicionales de seguridad que estén fuera del alcance de un plan de pruebas básico, como pruebas de vulnerabilidades, pruebas de penetración y análisis de código                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se probara los servicios soap obtenidos de la pagina http://webservices.oorsprong.org/websamples.countryinfo/CountryInfoService.wso?wsdl y https://www.crcind.com/csp/samples/SOAP.Demo.CLS?WSDL en donde se pondran a pruebas de diferentes maneras posibles en donde se listara y se haran busquedas por identificadores de personas </t>
+  </si>
+  <si>
+    <t>Definir los requisitos: Lo primero que debemos hacer es definir los requisitos del servicio SOAP. 
+Crear casos de prueba: Una vez que se han definido los requisitos, podemos crear casos de prueba. Los casos de prueba deben cubrir todas las funcionalidades definidas en los requisitos
+Diseñar los datos de prueba: Para probar el servicio SOAP
+Ejecutar pruebas: Una vez que se hayan creado los casos de prueba y los datos de prueba, podemos ejecutar las pruebas en el servicio SOAP                                     
+Documentar los resultados: Después de ejecutar las pruebas, es importante documentar los resultados
+Informar y rastrear problemas: Finalmente, debemos informar y rastrear cualquier problema encontrado durante las pruebas</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -522,6 +546,12 @@
       <sz val="10"/>
       <name val="SimSun"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -895,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -933,7 +963,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -962,6 +992,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -978,34 +1025,195 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="75">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1107,39 +1315,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF92D050"/>
           <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1314,172 +1489,36 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
+        <color rgb="FF92D050"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
+        <color rgb="FFFFFF00"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
+        <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2446,23 +2485,23 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_2" displayName="Table_2" ref="A7:M9">
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Consecutivo" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción Riesgo" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tipo de Riesgo" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Release" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Probabilidad de ocurrencia" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Impacto" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Riesgo" dataDxfId="35">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Consecutivo" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripción Riesgo" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tipo de Riesgo" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Release" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Probabilidad de ocurrencia" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Impacto" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Riesgo" dataDxfId="32">
       <calculatedColumnFormula>'Ejemplo Matriz de Riesgo'!$E$8:$E$9*'Ejemplo Matriz de Riesgo'!$F$8:$F$9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Riesgo " dataDxfId="34">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Riesgo " dataDxfId="31">
       <calculatedColumnFormula>'Ejemplo Matriz de Riesgo'!$G$8:$G$9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Acción" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Plan de Acción" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Responsable de la Acción" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Fecha Compromiso " dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Estado" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Acción" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Plan de Acción" dataDxfId="29"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Responsable de la Acción" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Fecha Compromiso " dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Estado" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="Ejemplo Matriz de Riesgo-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2471,8 +2510,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_4" displayName="Table_4" ref="A1:B5">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Plan de Acción" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Descripción" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Plan de Acción" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Descripción" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2481,7 +2520,7 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table_5" displayName="Table_5" ref="D1:D3">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Tipo de Riesg" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Tipo de Riesg" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2490,9 +2529,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table_6" displayName="Table_6" ref="F1:H6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Probabilidad" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Evaluación" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Definición" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Probabilidad" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Evaluación" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Definición" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2501,9 +2540,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table_7" displayName="Table_7" ref="J1:L6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Impacto" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Evaluación" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Definición" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Impacto" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Evaluación" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Definición" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2512,7 +2551,7 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table_8" displayName="Table_8" ref="A8:A10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Responsable Calidad" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Responsable Calidad" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2521,7 +2560,7 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table_9" displayName="Table_9" ref="D8:D10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Plan de Calidad" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Plan de Calidad" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2530,7 +2569,7 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table_10" displayName="Table_10" ref="F8:F10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Historia de Usuario" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Historia de Usuario" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2539,7 +2578,7 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table_11" displayName="Table_11" ref="A12:A14">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Estado" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Estado" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2748,8 +2787,8 @@
   </sheetPr>
   <dimension ref="A1:M1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2843,32 +2882,32 @@
       <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>14</v>
+      <c r="B8" s="53" t="s">
+        <v>110</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="53" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>22</v>
+      <c r="F8" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="I8" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>115</v>
       </c>
       <c r="K8" s="26" t="s">
         <v>23</v>
@@ -3942,8 +3981,8 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -5207,15 +5246,15 @@
     <mergeCell ref="A1:M6"/>
   </mergeCells>
   <conditionalFormatting sqref="H8:H9">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="between">
       <formula>20</formula>
       <formula>25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="2" operator="between">
       <formula>11</formula>
       <formula>19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>
@@ -5271,21 +5310,21 @@
     <row r="1" spans="2:5" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:5" ht="14.25" customHeight="1"/>
     <row r="3" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="49"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="41"/>
     </row>
     <row r="4" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="50"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="5" spans="2:5" ht="29.25" customHeight="1">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="48" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -5299,7 +5338,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="26.25" customHeight="1">
-      <c r="B6" s="38"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="10">
         <v>100</v>
       </c>
@@ -5312,7 +5351,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="32" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -5326,7 +5365,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B8" s="38"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="10">
         <v>100</v>
       </c>
@@ -5339,30 +5378,30 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="30" customHeight="1">
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="44"/>
       <c r="E9" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B10" s="38"/>
-      <c r="C10" s="34">
+      <c r="B10" s="49"/>
+      <c r="C10" s="45">
         <v>20</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="15">
         <f>C10</f>
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="50" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="12" t="s">
@@ -5376,7 +5415,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="30" customHeight="1">
-      <c r="B12" s="38"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="10">
         <v>1</v>
       </c>
@@ -5389,7 +5428,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="32" t="s">
         <v>61</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -5403,7 +5442,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B14" s="38"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="10">
         <v>50</v>
       </c>
@@ -5416,41 +5455,41 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="30" customHeight="1">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="33"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B16" s="41"/>
-      <c r="C16" s="35" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="17" t="str">
         <f>C16</f>
         <v>SI</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="44"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="36"/>
     </row>
     <row r="18" spans="2:5" ht="14.25" customHeight="1">
-      <c r="B18" s="41"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="2:5" ht="14.25" customHeight="1"/>
     <row r="20" spans="2:5" ht="14.25" customHeight="1"/>
@@ -6455,54 +6494,54 @@
     <mergeCell ref="B15:B16"/>
   </mergeCells>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="greaterThanOrEqual">
       <formula>95%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThanOrEqual">
       <formula>79%</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="between">
       <formula>80%</formula>
       <formula>94%</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="lessThanOrEqual">
       <formula>0.14</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="greaterThanOrEqual">
       <formula>0.15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="lessThanOrEqual">
       <formula>0.19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="greaterThanOrEqual">
       <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>